<commit_message>
update information about Kosovo
</commit_message>
<xml_diff>
--- a/regions/reviewed regions codes (flags, highcharts maps, drupal, FAO, names translated).xlsx
+++ b/regions/reviewed regions codes (flags, highcharts maps, drupal, FAO, names translated).xlsx
@@ -184,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N252" authorId="0" shapeId="0">
+    <comment ref="N253" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9675" uniqueCount="2309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9680" uniqueCount="2310">
   <si>
     <t>admin,C,254</t>
   </si>
@@ -7144,6 +7144,9 @@
   </si>
   <si>
     <t>Drupal label FR</t>
+  </si>
+  <si>
+    <t>XKX</t>
   </si>
 </sst>
 </file>
@@ -7906,7 +7909,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -7985,10 +7988,6 @@
     <xf numFmtId="0" fontId="30" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="153" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -8004,11 +8003,6 @@
     <xf numFmtId="0" fontId="28" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="187" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -9794,6 +9788,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7056120" cy="13289280"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10087,8 +10129,8 @@
   <dimension ref="A1:BM267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1:AA1"/>
+      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F251" sqref="F251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10139,143 +10181,143 @@
     <col min="49" max="49" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="41" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:49" s="39" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>2146</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="38" t="s">
         <v>2187</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="39" t="s">
         <v>2186</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>2200</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="39" t="s">
         <v>2202</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="39" t="s">
         <v>2185</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="39" t="s">
         <v>2204</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="39" t="s">
         <v>2203</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="39" t="s">
         <v>2305</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="39" t="s">
         <v>2308</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="39" t="s">
         <v>2307</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="39" t="s">
         <v>2306</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="39" t="s">
         <v>2205</v>
       </c>
-      <c r="N1" s="42" t="s">
+      <c r="N1" s="40" t="s">
         <v>2120</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="O1" s="38" t="s">
         <v>2133</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="P1" s="38" t="s">
         <v>2119</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="38" t="s">
         <v>2147</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="R1" s="38" t="s">
         <v>2134</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="S1" s="38" t="s">
         <v>2132</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="38" t="s">
         <v>2148</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="38" t="s">
         <v>2144</v>
       </c>
-      <c r="V1" s="40" t="s">
+      <c r="V1" s="38" t="s">
         <v>2143</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="W1" s="38" t="s">
         <v>2149</v>
       </c>
-      <c r="X1" s="40" t="s">
+      <c r="X1" s="38" t="s">
         <v>2150</v>
       </c>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40" t="s">
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="40" t="s">
+      <c r="AA1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="AB1" s="40" t="s">
+      <c r="AB1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="40" t="s">
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+      <c r="AF1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="40" t="s">
+      <c r="AG1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="AH1" s="40" t="s">
+      <c r="AH1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="AI1" s="40" t="s">
+      <c r="AI1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="AJ1" s="40" t="s">
+      <c r="AJ1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AK1" s="40" t="s">
+      <c r="AK1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="AL1" s="40" t="s">
+      <c r="AL1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AM1" s="40" t="s">
+      <c r="AM1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="AN1" s="40" t="s">
+      <c r="AN1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="AO1" s="40" t="s">
+      <c r="AO1" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="AP1" s="40" t="s">
+      <c r="AP1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="AQ1" s="40" t="s">
+      <c r="AQ1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="AR1" s="40" t="s">
+      <c r="AR1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="AS1" s="44" t="s">
+      <c r="AS1" s="42" t="s">
         <v>1912</v>
       </c>
-      <c r="AT1" s="40" t="s">
+      <c r="AT1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="AU1" s="40" t="s">
+      <c r="AU1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="AV1" s="40" t="s">
+      <c r="AV1" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="AW1" s="40" t="s">
+      <c r="AW1" s="38" t="s">
         <v>18</v>
       </c>
     </row>
@@ -10425,11 +10467,11 @@
       <c r="C3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="48" t="s">
         <v>34</v>
       </c>
       <c r="E3" s="18"/>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="48" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="18" t="b">
@@ -19627,7 +19669,7 @@
       <c r="H70" s="18" t="s">
         <v>1470</v>
       </c>
-      <c r="I70" s="52" t="s">
+      <c r="I70" s="47" t="s">
         <v>1466</v>
       </c>
       <c r="J70" s="14" t="s">
@@ -44539,291 +44581,263 @@
         <v>48</v>
       </c>
     </row>
-    <row r="251" spans="1:49" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A251" s="45"/>
-      <c r="B251" s="45"/>
-      <c r="G251" s="45"/>
-      <c r="H251" s="45"/>
-      <c r="I251" s="46"/>
-      <c r="J251" s="46"/>
-      <c r="K251" s="46"/>
-      <c r="L251" s="46"/>
-      <c r="M251" s="45"/>
-      <c r="N251" s="45"/>
-      <c r="O251" s="12"/>
-      <c r="P251" s="12"/>
-      <c r="R251" s="12"/>
-      <c r="S251" s="47"/>
-      <c r="T251" s="38"/>
-      <c r="U251" s="12"/>
-      <c r="V251" s="12"/>
-      <c r="W251" s="38"/>
-      <c r="X251" s="12"/>
-      <c r="Y251" s="12"/>
-      <c r="Z251" s="18"/>
-      <c r="AA251" s="18"/>
-      <c r="AB251" s="38"/>
-      <c r="AD251" s="39"/>
-      <c r="AE251" s="39"/>
-      <c r="AF251" s="12"/>
-      <c r="AG251" s="12"/>
-      <c r="AH251" s="12"/>
-      <c r="AI251" s="12"/>
-      <c r="AJ251" s="12"/>
-      <c r="AK251" s="12"/>
-      <c r="AL251" s="12"/>
-      <c r="AM251" s="12"/>
-      <c r="AN251" s="12"/>
-      <c r="AO251" s="12"/>
-      <c r="AP251" s="12"/>
-      <c r="AQ251" s="12"/>
-      <c r="AR251" s="12"/>
-      <c r="AT251" s="14"/>
-      <c r="AU251" s="12"/>
-      <c r="AV251" s="12"/>
-      <c r="AW251" s="12"/>
+    <row r="251" spans="1:49" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F251" s="21" t="s">
+        <v>1971</v>
+      </c>
+      <c r="G251" s="21" t="s">
+        <v>2183</v>
+      </c>
+      <c r="H251" s="21" t="s">
+        <v>2309</v>
+      </c>
+      <c r="I251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="J251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="K251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="L251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="Q251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="T251" s="21" t="s">
+        <v>1932</v>
+      </c>
+      <c r="W251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="Z251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="AA251" s="21" t="s">
+        <v>1932</v>
+      </c>
+      <c r="AB251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="AF251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="AG251" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="AH251" s="21" t="s">
+        <v>961</v>
+      </c>
+      <c r="AJ251" s="21" t="s">
+        <v>962</v>
+      </c>
+      <c r="AK251" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL251" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM251" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN251" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO251" s="21" t="s">
+        <v>963</v>
+      </c>
+      <c r="AP251" s="21" t="s">
+        <v>964</v>
+      </c>
+      <c r="AQ251" s="21" t="s">
+        <v>965</v>
+      </c>
+      <c r="AR251" s="21" t="s">
+        <v>961</v>
+      </c>
+      <c r="AT251" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU251" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV251" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW251" s="21" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="252" spans="1:49" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C252" s="21" t="s">
+    <row r="252" spans="1:49" s="18" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:49" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C253" s="21" t="s">
         <v>1961</v>
       </c>
-      <c r="D252" s="21" t="s">
+      <c r="D253" s="21" t="s">
         <v>2188</v>
       </c>
-      <c r="E252" s="21" t="s">
+      <c r="E253" s="21" t="s">
         <v>2201</v>
       </c>
-      <c r="N252" s="21" t="s">
+      <c r="N253" s="21" t="s">
         <v>1961</v>
       </c>
-      <c r="P252" s="21" t="s">
+      <c r="P253" s="21" t="s">
         <v>1962</v>
       </c>
-      <c r="Q252" s="21" t="s">
+      <c r="Q253" s="21" t="s">
         <v>1962</v>
       </c>
-      <c r="S252" s="21" t="s">
+      <c r="S253" s="21" t="s">
         <v>1963</v>
       </c>
-      <c r="V252" s="21" t="s">
+      <c r="V253" s="21" t="s">
         <v>1964</v>
       </c>
-      <c r="AA252" s="21" t="s">
+      <c r="AA253" s="21" t="s">
         <v>1963</v>
       </c>
-      <c r="AB252" s="21" t="s">
+      <c r="AB253" s="21" t="s">
         <v>1964</v>
       </c>
     </row>
-    <row r="253" spans="1:49" x14ac:dyDescent="0.3">
-      <c r="A253" s="18"/>
-      <c r="B253" s="18"/>
-      <c r="C253" s="18"/>
-      <c r="G253" s="18"/>
-      <c r="H253" s="18"/>
-      <c r="M253" s="18"/>
-      <c r="O253" s="2"/>
-      <c r="P253" s="2"/>
-      <c r="Q253" s="1"/>
-      <c r="R253" s="2"/>
-      <c r="T253" s="1"/>
-      <c r="U253" s="2"/>
-      <c r="V253" s="2"/>
-      <c r="W253" s="2"/>
-      <c r="X253" s="2"/>
-      <c r="Y253" s="2"/>
-      <c r="AD253" s="19"/>
-      <c r="AE253" s="19"/>
-      <c r="AF253" s="2"/>
-      <c r="AG253" s="2"/>
-      <c r="AH253" s="2"/>
-      <c r="AI253" s="2"/>
-      <c r="AJ253" s="2"/>
-      <c r="AK253" s="2"/>
-      <c r="AL253" s="2"/>
-      <c r="AM253" s="2"/>
-      <c r="AN253" s="2"/>
-      <c r="AO253" s="2"/>
-      <c r="AP253" s="2"/>
-      <c r="AQ253" s="2"/>
-      <c r="AR253" s="2"/>
-      <c r="AT253" s="2"/>
-      <c r="AU253" s="2"/>
-      <c r="AV253" s="2"/>
-      <c r="AW253" s="2"/>
+    <row r="254" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A254" s="18"/>
+      <c r="B254" s="18"/>
+      <c r="C254" s="18"/>
+      <c r="G254" s="18"/>
+      <c r="H254" s="18"/>
+      <c r="M254" s="18"/>
+      <c r="O254" s="2"/>
+      <c r="P254" s="2"/>
+      <c r="Q254" s="1"/>
+      <c r="R254" s="2"/>
+      <c r="T254" s="1"/>
+      <c r="U254" s="2"/>
+      <c r="V254" s="2"/>
+      <c r="W254" s="2"/>
+      <c r="X254" s="2"/>
+      <c r="Y254" s="2"/>
+      <c r="AD254" s="19"/>
+      <c r="AE254" s="19"/>
+      <c r="AF254" s="2"/>
+      <c r="AG254" s="2"/>
+      <c r="AH254" s="2"/>
+      <c r="AI254" s="2"/>
+      <c r="AJ254" s="2"/>
+      <c r="AK254" s="2"/>
+      <c r="AL254" s="2"/>
+      <c r="AM254" s="2"/>
+      <c r="AN254" s="2"/>
+      <c r="AO254" s="2"/>
+      <c r="AP254" s="2"/>
+      <c r="AQ254" s="2"/>
+      <c r="AR254" s="2"/>
+      <c r="AT254" s="2"/>
+      <c r="AU254" s="2"/>
+      <c r="AV254" s="2"/>
+      <c r="AW254" s="2"/>
     </row>
-    <row r="254" spans="1:49" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="Q254" s="21" t="s">
+    <row r="255" spans="1:49" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q255" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="T254" s="21" t="s">
+      <c r="T255" s="21" t="s">
         <v>1915</v>
       </c>
-      <c r="W254" s="21" t="s">
+      <c r="W255" s="21" t="s">
         <v>1916</v>
       </c>
-      <c r="Z254" s="21" t="s">
+      <c r="Z255" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="AA254" s="21" t="s">
+      <c r="AA255" s="21" t="s">
         <v>1915</v>
       </c>
-      <c r="AB254" s="21" t="s">
+      <c r="AB255" s="21" t="s">
         <v>1916</v>
       </c>
-      <c r="AF254" s="21" t="s">
+      <c r="AF255" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="AG254" s="21" t="s">
+      <c r="AG255" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="AH254" s="21" t="s">
+      <c r="AH255" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="AJ254" s="21" t="s">
+      <c r="AJ255" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="AK254" s="21">
+      <c r="AK255" s="21">
         <v>-99</v>
       </c>
-      <c r="AL254" s="21">
+      <c r="AL255" s="21">
         <v>-99</v>
       </c>
-      <c r="AM254" s="21">
+      <c r="AM255" s="21">
         <v>36</v>
       </c>
-      <c r="AN254" s="21">
+      <c r="AN255" s="21">
         <v>-99</v>
       </c>
-      <c r="AO254" s="21">
+      <c r="AO255" s="21">
         <v>-99</v>
       </c>
-      <c r="AP254" s="21">
+      <c r="AP255" s="21">
         <v>-99</v>
       </c>
-      <c r="AQ254" s="21" t="s">
+      <c r="AQ255" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="AR254" s="21" t="s">
+      <c r="AR255" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="AT254" s="21" t="s">
+      <c r="AT255" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="AU254" s="21" t="s">
+      <c r="AU255" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="AV254" s="21" t="s">
+      <c r="AV255" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="AW254" s="21" t="s">
+      <c r="AW255" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="255" spans="1:49" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="Q255" s="21" t="s">
+    <row r="256" spans="1:49" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q256" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="T255" s="21" t="s">
+      <c r="T256" s="21" t="s">
         <v>1919</v>
       </c>
-      <c r="W255" s="21" t="s">
+      <c r="W256" s="21" t="s">
         <v>1920</v>
       </c>
-      <c r="Z255" s="21" t="s">
+      <c r="Z256" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="AA255" s="21" t="s">
+      <c r="AA256" s="21" t="s">
         <v>1919</v>
       </c>
-      <c r="AB255" s="21" t="s">
+      <c r="AB256" s="21" t="s">
         <v>1920</v>
       </c>
-      <c r="AF255" s="21" t="s">
+      <c r="AF256" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="AG255" s="21" t="s">
+      <c r="AG256" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="AH255" s="21" t="s">
+      <c r="AH256" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="AJ255" s="21" t="s">
+      <c r="AJ256" s="21" t="s">
         <v>361</v>
-      </c>
-      <c r="AK255" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL255" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM255" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN255" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="AO255" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="AP255" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ255" s="21" t="s">
-        <v>465</v>
-      </c>
-      <c r="AR255" s="21" t="s">
-        <v>465</v>
-      </c>
-      <c r="AT255" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU255" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV255" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="AW255" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="256" spans="1:49" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F256" s="21" t="s">
-        <v>1971</v>
-      </c>
-      <c r="G256" s="21" t="s">
-        <v>2183</v>
-      </c>
-      <c r="Q256" s="21" t="s">
-        <v>960</v>
-      </c>
-      <c r="T256" s="21" t="s">
-        <v>1932</v>
-      </c>
-      <c r="W256" s="21" t="s">
-        <v>960</v>
-      </c>
-      <c r="Z256" s="21" t="s">
-        <v>960</v>
-      </c>
-      <c r="AA256" s="21" t="s">
-        <v>1932</v>
-      </c>
-      <c r="AB256" s="21" t="s">
-        <v>960</v>
-      </c>
-      <c r="AF256" s="21" t="s">
-        <v>960</v>
-      </c>
-      <c r="AG256" s="21" t="s">
-        <v>960</v>
-      </c>
-      <c r="AH256" s="21" t="s">
-        <v>961</v>
-      </c>
-      <c r="AJ256" s="21" t="s">
-        <v>962</v>
       </c>
       <c r="AK256" s="21" t="s">
         <v>54</v>
@@ -44838,25 +44852,25 @@
         <v>128</v>
       </c>
       <c r="AO256" s="21" t="s">
-        <v>963</v>
+        <v>54</v>
       </c>
       <c r="AP256" s="21" t="s">
-        <v>964</v>
+        <v>54</v>
       </c>
       <c r="AQ256" s="21" t="s">
-        <v>965</v>
+        <v>465</v>
       </c>
       <c r="AR256" s="21" t="s">
-        <v>961</v>
+        <v>465</v>
       </c>
       <c r="AT256" s="21" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="AU256" s="21" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="AV256" s="21" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="AW256" s="21" t="s">
         <v>65</v>
@@ -45166,7 +45180,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="36"/>
@@ -45187,7 +45201,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="44" t="s">
         <v>2220</v>
       </c>
       <c r="B2" s="37"/>
@@ -45206,7 +45220,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="44" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="37"/>
@@ -45227,7 +45241,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="36"/>
@@ -45248,7 +45262,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="43" t="s">
         <v>134</v>
       </c>
       <c r="B5" s="36"/>
@@ -45269,7 +45283,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="44" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="37"/>
@@ -45290,7 +45304,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="43" t="s">
         <v>265</v>
       </c>
       <c r="B7" s="36"/>
@@ -45311,7 +45325,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="44" t="s">
         <v>911</v>
       </c>
       <c r="B8" s="37"/>
@@ -45332,7 +45346,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="44" t="s">
         <v>2237</v>
       </c>
       <c r="B9" s="37"/>
@@ -45351,7 +45365,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="44" t="s">
         <v>176</v>
       </c>
       <c r="B10" s="37"/>
@@ -45372,7 +45386,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="43" t="s">
         <v>363</v>
       </c>
       <c r="B11" s="36"/>
@@ -45393,7 +45407,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="44" t="s">
         <v>216</v>
       </c>
       <c r="B12" s="37"/>
@@ -45414,7 +45428,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="43" t="s">
         <v>2248</v>
       </c>
       <c r="B13" s="36"/>
@@ -45433,7 +45447,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="43" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="36"/>
@@ -45454,7 +45468,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="45" t="s">
         <v>2251</v>
       </c>
       <c r="B15" s="37"/>
@@ -45475,7 +45489,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="44" t="s">
         <v>960</v>
       </c>
       <c r="B16" s="37"/>
@@ -45494,7 +45508,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="43" t="s">
         <v>2252</v>
       </c>
       <c r="B17" s="36"/>
@@ -45515,7 +45529,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="44" t="s">
         <v>602</v>
       </c>
       <c r="B18" s="37"/>
@@ -45536,7 +45550,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="43" t="s">
         <v>2258</v>
       </c>
       <c r="B19" s="36"/>
@@ -45557,7 +45571,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="46" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="36"/>
@@ -45578,7 +45592,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="44" t="s">
         <v>535</v>
       </c>
       <c r="B21" s="37"/>
@@ -45599,7 +45613,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="43" t="s">
         <v>273</v>
       </c>
       <c r="B22" s="36"/>
@@ -45620,7 +45634,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="43" t="s">
         <v>73</v>
       </c>
       <c r="B23" s="36"/>
@@ -45641,7 +45655,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="44" t="s">
         <v>119</v>
       </c>
       <c r="B24" s="37"/>
@@ -45662,7 +45676,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="44" t="s">
         <v>120</v>
       </c>
       <c r="B25" s="37"/>
@@ -45683,7 +45697,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="44" t="s">
         <v>2278</v>
       </c>
       <c r="B26" s="37"/>
@@ -45702,7 +45716,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="44" t="s">
         <v>102</v>
       </c>
       <c r="B27" s="37"/>
@@ -45723,7 +45737,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="43" t="s">
         <v>304</v>
       </c>
       <c r="B28" s="36"/>
@@ -45744,7 +45758,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="44" t="s">
         <v>321</v>
       </c>
       <c r="B29" s="37"/>
@@ -45765,7 +45779,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="44" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="37"/>
@@ -45786,7 +45800,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="44" t="s">
         <v>64</v>
       </c>
       <c r="B31" s="37"/>
@@ -45807,7 +45821,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B32" s="36"/>
@@ -45828,7 +45842,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="43" t="s">
         <v>2295</v>
       </c>
       <c r="B33" s="36"/>
@@ -45847,7 +45861,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="43" t="s">
         <v>195</v>
       </c>
       <c r="B34" s="36"/>
@@ -45868,7 +45882,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="44" t="s">
         <v>92</v>
       </c>
       <c r="B35" s="37"/>
@@ -45889,7 +45903,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="43" t="s">
         <v>159</v>
       </c>
       <c r="B36" s="36"/>

</xml_diff>

<commit_message>
updated name of Laos
</commit_message>
<xml_diff>
--- a/regions/reviewed regions codes (flags, highcharts maps, drupal, FAO, names translated).xlsx
+++ b/regions/reviewed regions codes (flags, highcharts maps, drupal, FAO, names translated).xlsx
@@ -9836,6 +9836,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7056120" cy="13289280"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10129,8 +10177,8 @@
   <dimension ref="A1:BM267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F251" sqref="F251"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27322,13 +27370,13 @@
         <v>975</v>
       </c>
       <c r="I126" s="22" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="J126" s="22" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="K126" s="22" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="L126" s="22" t="s">
         <v>974</v>

</xml_diff>